<commit_message>
Add conf matrix saving to get_train_stats; Add plot_confusion_matrix to vis_functions; Upd reports
</commit_message>
<xml_diff>
--- a/reports/evaluation_results.xlsx
+++ b/reports/evaluation_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto Final\Projeto Petrobras\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB17F0-33EE-41D8-B5E6-7D0290545CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CD3ACC-E71F-4C1E-82E2-3A408CF01977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Loss</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Runs</t>
+  </si>
+  <si>
+    <t>Ref val certo</t>
+  </si>
+  <si>
+    <t>Errado</t>
   </si>
 </sst>
 </file>
@@ -68,9 +74,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +107,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -198,26 +211,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -263,24 +304,59 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,36 +637,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H12"/>
+  <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
@@ -603,154 +680,215 @@
       <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="27">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="14">
         <v>0.23726000000000003</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="15">
         <v>1.8827001885589754E-2</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="9">
         <v>0.90593159999999995</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="23">
         <v>0.01</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="E8" s="29">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F8" s="30">
+        <v>0.88344</v>
+      </c>
+      <c r="G8" s="31">
+        <v>1.491E-2</v>
+      </c>
+      <c r="H8" s="7">
         <v>5</v>
       </c>
-      <c r="D8" s="19">
+    </row>
+    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16">
         <v>0.159</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E9" s="17">
         <v>0.01</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F9" s="10">
         <v>0.93700000000000006</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G9" s="24">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H9" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="26">
+    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="27">
         <v>2</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D10" s="18">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E10" s="15">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F10" s="11">
         <v>0.95199999999999996</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G10" s="23">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H10" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="8" t="s">
+    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="36">
+        <v>2.681</v>
+      </c>
+      <c r="E11" s="37">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="F11" s="38">
+        <v>0.33962999999999999</v>
+      </c>
+      <c r="G11" s="39">
+        <v>5.4350000000000002E-2</v>
+      </c>
+      <c r="H11" s="40">
         <v>5</v>
       </c>
-      <c r="D10" s="22">
+      <c r="I11" s="41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="19">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E12" s="20">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F12" s="12">
         <v>0.94299999999999995</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G12" s="25">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H12" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="26">
+    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="27">
         <v>3</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C13" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D13" s="14">
         <v>1.0760000000000001</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E13" s="15">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F13" s="9">
         <v>0.65500000000000003</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G13" s="23">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H13" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="8" t="s">
+    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="7">
         <v>5</v>
       </c>
-      <c r="D12" s="24">
+    </row>
+    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="21">
         <v>0.49299999999999999</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E15" s="22">
         <v>5.5E-2</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F15" s="13">
         <v>0.68200000000000005</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G15" s="26">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A7:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Upd reports with new val set results
</commit_message>
<xml_diff>
--- a/reports/evaluation_results.xlsx
+++ b/reports/evaluation_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B80F4B4-5D54-4257-AB2D-82EDA95EC2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D47ECF1-183B-4E6E-87E7-3A0488435B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,7 +639,7 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Upd reports with semiauto dataset with ref val
</commit_message>
<xml_diff>
--- a/reports/evaluation_results.xlsx
+++ b/reports/evaluation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D47ECF1-183B-4E6E-87E7-3A0488435B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E06C41-9F42-45E1-802D-32B28EE0636E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>Loss</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Acc Std</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Semiauto</t>
-  </si>
-  <si>
     <t>Resnet18_sqrt_weights_25_epochs</t>
   </si>
   <si>
@@ -62,10 +56,19 @@
     <t>Runs</t>
   </si>
   <si>
-    <t>Ref val certo</t>
+    <t>Errado</t>
   </si>
   <si>
-    <t>Errado</t>
+    <t>Ref val semiauto</t>
+  </si>
+  <si>
+    <t>Ref val ref</t>
+  </si>
+  <si>
+    <t>Semiauto val semiauto</t>
+  </si>
+  <si>
+    <t>Semiauto val ref</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -248,11 +251,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -273,9 +338,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -297,12 +359,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -310,9 +366,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -355,6 +408,105 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,37 +788,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.453125" customWidth="1"/>
     <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="10" max="10" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.36328125" customWidth="1"/>
+    <col min="12" max="12" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
@@ -680,224 +838,560 @@
         <v>3</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="39">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="P6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="35">
+        <v>1</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="12">
         <v>0.23726000000000003</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>1.8827001885589754E-2</v>
       </c>
       <c r="F7" s="8">
         <v>0.90593159999999995</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="19">
         <v>0.01</v>
       </c>
       <c r="H7" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="30" t="s">
+      <c r="J7" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="35">
+        <v>1</v>
+      </c>
+      <c r="L7" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="18">
+      <c r="M7" s="12">
+        <v>0.23726000000000003</v>
+      </c>
+      <c r="N7" s="13">
+        <v>1.8827001885589754E-2</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.90593159999999995</v>
+      </c>
+      <c r="P7" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="Q7" s="42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="36"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="17">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="22">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="23">
         <v>0.88344</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="24">
         <v>1.491E-2</v>
       </c>
       <c r="H8" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="J8" s="36"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="37">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="N8" s="38">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O8" s="39">
+        <v>0.91352999999999995</v>
+      </c>
+      <c r="P8" s="21">
+        <v>9.2099999999999994E-3</v>
+      </c>
+      <c r="Q8" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="36"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="37">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="E9" s="38">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F9" s="39">
+        <v>0.91352999999999995</v>
+      </c>
+      <c r="G9" s="21">
+        <v>9.2099999999999994E-3</v>
+      </c>
+      <c r="H9" s="7">
+        <v>5</v>
+      </c>
+      <c r="J9" s="36"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="60">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="N9" s="61">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="O9" s="62">
+        <v>0.88344</v>
+      </c>
+      <c r="P9" s="63">
+        <v>1.491E-2</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="36"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14">
         <v>0.159</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E10" s="15">
         <v>0.01</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F10" s="9">
         <v>0.93700000000000006</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G10" s="20">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H9" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="39">
+      <c r="H10" s="7">
+        <v>5</v>
+      </c>
+      <c r="J10" s="36"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0.159</v>
+      </c>
+      <c r="N10" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="P10" s="20">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q10" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="36"/>
+      <c r="B11" s="35">
         <v>2</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="17">
+      <c r="C11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="16">
         <v>0.13800000000000001</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E11" s="13">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F11" s="10">
         <v>0.95199999999999996</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G11" s="19">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H11" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="40"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="32" t="s">
+      <c r="J11" s="36"/>
+      <c r="K11" s="35">
+        <v>2</v>
+      </c>
+      <c r="L11" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="33">
+      <c r="M11" s="64">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="N11" s="65">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O11" s="66">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="P11" s="67">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Q11" s="42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="36"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="29">
         <v>2.681</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E12" s="30">
         <v>0.23899999999999999</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F12" s="31">
         <v>0.33962999999999999</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G12" s="32">
         <v>5.4350000000000002E-2</v>
       </c>
-      <c r="H11" s="37">
-        <v>5</v>
-      </c>
-      <c r="I11" s="38" t="s">
+      <c r="H12" s="33">
+        <v>5</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="29">
+        <v>4.5330000000000004</v>
+      </c>
+      <c r="N12" s="30">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="O12" s="31">
+        <v>0.12762999999999999</v>
+      </c>
+      <c r="P12" s="32">
+        <v>2.589E-2</v>
+      </c>
+      <c r="Q12" s="44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="36"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="29">
+        <v>4.5330000000000004</v>
+      </c>
+      <c r="E13" s="30">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.12762999999999999</v>
+      </c>
+      <c r="G13" s="32">
+        <v>2.589E-2</v>
+      </c>
+      <c r="H13" s="33">
+        <v>5</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="36"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="50">
+        <v>2.681</v>
+      </c>
+      <c r="N13" s="51">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="O13" s="52">
+        <v>0.33962999999999999</v>
+      </c>
+      <c r="P13" s="53">
+        <v>5.4350000000000002E-2</v>
+      </c>
+      <c r="Q13" s="44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="36"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="18">
+      <c r="D14" s="17">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E14" s="18">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F14" s="11">
         <v>0.94299999999999995</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G14" s="21">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H12" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="39">
+      <c r="H14" s="7">
+        <v>5</v>
+      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="68">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="N14" s="69">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="O14" s="70">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="P14" s="71">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Q14" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="36"/>
+      <c r="B15" s="35">
         <v>3</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="13">
+      <c r="C15" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="16">
         <v>1.0760000000000001</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E15" s="40">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F15" s="10">
         <v>0.65500000000000003</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G15" s="41">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H15" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="30" t="s">
+      <c r="J15" s="36"/>
+      <c r="K15" s="35">
+        <v>3</v>
+      </c>
+      <c r="L15" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="18">
+      <c r="M15" s="16">
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="N15" s="40">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="P15" s="41">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="Q15" s="42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="36"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="17">
         <v>1.64</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E16" s="22">
         <v>0.22800000000000001</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F16" s="23">
         <v>0.53088999999999997</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G16" s="24">
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="H14" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="20">
+      <c r="H16" s="7">
+        <v>5</v>
+      </c>
+      <c r="J16" s="36"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="55">
+        <v>1.528</v>
+      </c>
+      <c r="N16" s="56">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="O16" s="57">
+        <v>0.54876999999999998</v>
+      </c>
+      <c r="P16" s="58">
+        <v>5.262E-2</v>
+      </c>
+      <c r="Q16" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="36"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="17">
+        <v>1.528</v>
+      </c>
+      <c r="E17" s="22">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.54876999999999998</v>
+      </c>
+      <c r="G17" s="24">
+        <v>5.262E-2</v>
+      </c>
+      <c r="H17" s="7">
+        <v>5</v>
+      </c>
+      <c r="J17" s="36"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="17">
+        <v>1.64</v>
+      </c>
+      <c r="N17" s="22">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="O17" s="23">
+        <v>0.53088999999999997</v>
+      </c>
+      <c r="P17" s="24">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="Q17" s="42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="36"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="14">
         <v>0.49299999999999999</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E18" s="15">
         <v>5.5E-2</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F18" s="9">
         <v>0.68200000000000005</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G18" s="20">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H18" s="7">
+        <v>5</v>
+      </c>
+      <c r="J18" s="36"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="N18" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="P18" s="20">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="Q18" s="42">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A7:A15"/>
+  <mergeCells count="8">
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="K11:K14"/>
+    <mergeCell ref="K15:K18"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A7:A18"/>
+    <mergeCell ref="J7:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Upd reports/evaluation_results w/ all entries
</commit_message>
<xml_diff>
--- a/reports/evaluation_results.xlsx
+++ b/reports/evaluation_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto Final\Projeto Petrobras\semiauto-video-annotation\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D372606-DC9D-49E4-9919-1C9A60AEE062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917446E-818C-4105-B32A-7D21E080383B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +120,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -283,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,18 +343,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -366,16 +361,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -409,16 +400,32 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -427,26 +434,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -732,37 +732,37 @@
   <dimension ref="A2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D6" s="3" t="s">
         <v>0</v>
       </c>
@@ -779,14 +779,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="54">
         <v>1</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="10">
@@ -801,58 +801,58 @@
       <c r="G7" s="16">
         <v>1.2460000000000001E-2</v>
       </c>
-      <c r="H7" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="53"/>
       <c r="B8" s="54"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="23">
         <v>0.19900000000000001</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="24">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="25">
         <v>0.91352999999999995</v>
       </c>
       <c r="G8" s="18">
         <v>9.2099999999999994E-3</v>
       </c>
-      <c r="H8" s="33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="53"/>
       <c r="B9" s="54"/>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="39">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="40">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="41">
         <v>0.88344</v>
       </c>
-      <c r="G9" s="48">
+      <c r="G9" s="42">
         <v>1.491E-2</v>
       </c>
-      <c r="H9" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="53"/>
       <c r="B10" s="54"/>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="32" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="12">
@@ -867,152 +867,152 @@
       <c r="G10" s="17">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H10" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="53"/>
       <c r="B11" s="54">
         <v>2</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E11" s="50">
+      <c r="E11" s="43">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="9">
         <v>0.94450000000000001</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="44">
         <v>1.1429999999999999E-2</v>
       </c>
-      <c r="H11" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="53"/>
       <c r="B12" s="54"/>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="22">
-        <v>4.5330000000000004</v>
-      </c>
-      <c r="E12" s="23">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="F12" s="24">
-        <v>0.12762999999999999</v>
-      </c>
-      <c r="G12" s="25">
-        <v>2.589E-2</v>
-      </c>
-      <c r="H12" s="34">
-        <v>5</v>
-      </c>
-      <c r="I12" s="26"/>
-    </row>
-    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="56">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="E12" s="58">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F12" s="57">
+        <v>0.88936999999999999</v>
+      </c>
+      <c r="G12" s="59">
+        <v>7.3099999999999997E-3</v>
+      </c>
+      <c r="H12" s="50">
+        <v>5</v>
+      </c>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="53"/>
       <c r="B13" s="54"/>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="46">
         <v>0.42399999999999999</v>
       </c>
-      <c r="E13" s="57">
+      <c r="E13" s="47">
         <v>3.9E-2</v>
       </c>
-      <c r="F13" s="58">
+      <c r="F13" s="48">
         <v>0.78874999999999995</v>
       </c>
-      <c r="G13" s="59">
+      <c r="G13" s="49">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H13" s="60">
-        <v>5</v>
-      </c>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="50">
+        <v>5</v>
+      </c>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="53"/>
       <c r="B14" s="54"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="32" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="12">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E14" s="61">
+      <c r="E14" s="51">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F14" s="62">
+      <c r="F14" s="52">
         <v>0.94299999999999995</v>
       </c>
       <c r="G14" s="17">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H14" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="53"/>
       <c r="B15" s="54">
         <v>3</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="14">
         <v>1.157</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="26">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F15" s="9">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="27">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="H15" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="53"/>
       <c r="B16" s="54"/>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="34">
         <v>1.528</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="35">
         <v>9.8299999999999998E-2</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="36">
         <v>0.54876999999999998</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="37">
         <v>5.262E-2</v>
       </c>
-      <c r="H16" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="53"/>
       <c r="B17" s="54"/>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="31" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="15">
@@ -1027,14 +1027,14 @@
       <c r="G17" s="21">
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="H17" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="53"/>
       <c r="B18" s="54"/>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="32" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="12">
@@ -1049,7 +1049,7 @@
       <c r="G18" s="17">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="28">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upd reports: Add semiauto_dataset_class_distributions; Rename semiauto_class_distributions to semiauto_annotations_class...
</commit_message>
<xml_diff>
--- a/reports/evaluation_results.xlsx
+++ b/reports/evaluation_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Arquivos Incomuns\Projeto Final\semiauto-video-annotation\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projeto Final\Projeto Petrobras\semiauto-video-annotation\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917446E-818C-4105-B32A-7D21E080383B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A17A69-D4DE-443A-A8ED-CCC8281B7709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Loss</t>
-  </si>
-  <si>
-    <t>Acc</t>
   </si>
   <si>
     <t>Loss Std</t>
@@ -56,16 +53,25 @@
     <t>Runs</t>
   </si>
   <si>
-    <t>Ref val semiauto</t>
+    <t>Dataset</t>
   </si>
   <si>
-    <t>Ref val ref</t>
+    <t>Validation Set</t>
   </si>
   <si>
-    <t>Semiauto val semiauto</t>
+    <t>Reference</t>
   </si>
   <si>
-    <t>Semiauto val ref</t>
+    <t>Semiauto</t>
+  </si>
+  <si>
+    <t>Avg Acc</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -76,7 +82,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,13 +107,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -121,7 +120,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -136,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -286,125 +318,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -421,33 +458,101 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -729,327 +834,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I18"/>
+  <dimension ref="A2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="A6" sqref="A6:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D5" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="B7" s="13">
         <v>1</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+      <c r="C7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.89100999999999997</v>
+      </c>
+      <c r="H7" s="19">
+        <v>1.2460000000000001E-2</v>
+      </c>
+      <c r="I7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="54">
-        <v>1</v>
-      </c>
-      <c r="C7" s="30" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="E7" s="11">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0.89100999999999997</v>
-      </c>
-      <c r="G7" s="16">
-        <v>1.2460000000000001E-2</v>
-      </c>
-      <c r="H7" s="28">
+      <c r="E8" s="22">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F8" s="23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0.91352999999999995</v>
+      </c>
+      <c r="H8" s="25">
+        <v>9.2099999999999994E-3</v>
+      </c>
+      <c r="I8" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="23">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="E8" s="24">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="F8" s="25">
-        <v>0.91352999999999995</v>
-      </c>
-      <c r="G8" s="18">
-        <v>9.2099999999999994E-3</v>
-      </c>
-      <c r="H8" s="29">
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="F9" s="29">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G9" s="30">
+        <v>0.88344</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1.491E-2</v>
+      </c>
+      <c r="I9" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="39">
-        <v>0.26800000000000002</v>
-      </c>
-      <c r="E9" s="40">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F9" s="41">
-        <v>0.88344</v>
-      </c>
-      <c r="G9" s="42">
-        <v>1.491E-2</v>
-      </c>
-      <c r="H9" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="34">
         <v>0.159</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="35">
         <v>0.01</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G10" s="36">
         <v>0.93700000000000006</v>
       </c>
-      <c r="G10" s="17">
+      <c r="H10" s="37">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H10" s="28">
+      <c r="I10" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54">
+    <row r="11" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13">
         <v>2</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="39">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E11" s="43">
+      <c r="F11" s="17">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F11" s="9">
+      <c r="G11" s="40">
         <v>0.94450000000000001</v>
       </c>
-      <c r="G11" s="44">
+      <c r="H11" s="19">
         <v>1.1429999999999999E-2</v>
       </c>
-      <c r="H11" s="28">
+      <c r="I11" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="56">
+    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="41">
         <v>0.29099999999999998</v>
       </c>
-      <c r="E12" s="58">
+      <c r="F12" s="42">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F12" s="57">
+      <c r="G12" s="43">
         <v>0.88936999999999999</v>
       </c>
-      <c r="G12" s="59">
+      <c r="H12" s="44">
         <v>7.3099999999999997E-3</v>
       </c>
-      <c r="H12" s="50">
+      <c r="I12" s="7">
         <v>5</v>
       </c>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="53"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="46">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="45">
         <v>0.42399999999999999</v>
       </c>
-      <c r="E13" s="47">
+      <c r="F13" s="46">
         <v>3.9E-2</v>
       </c>
-      <c r="F13" s="48">
+      <c r="G13" s="47">
         <v>0.78874999999999995</v>
       </c>
-      <c r="G13" s="49">
+      <c r="H13" s="48">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="H13" s="50">
+      <c r="I13" s="7">
         <v>5</v>
       </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="32" t="s">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="34">
         <v>0.14399999999999999</v>
       </c>
-      <c r="E14" s="51">
+      <c r="F14" s="50">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="F14" s="52">
+      <c r="G14" s="51">
         <v>0.94299999999999995</v>
       </c>
-      <c r="G14" s="17">
+      <c r="H14" s="37">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H14" s="28">
+      <c r="I14" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="53"/>
-      <c r="B15" s="54">
+    <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13">
         <v>3</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="39">
         <v>1.157</v>
       </c>
-      <c r="E15" s="26">
+      <c r="F15" s="52">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F15" s="9">
+      <c r="G15" s="40">
         <v>0.63200000000000001</v>
       </c>
-      <c r="G15" s="27">
+      <c r="H15" s="53">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="H15" s="28">
+      <c r="I15" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="53"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="34">
+    <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="55">
         <v>1.528</v>
       </c>
-      <c r="E16" s="35">
+      <c r="F16" s="56">
         <v>9.8299999999999998E-2</v>
       </c>
-      <c r="F16" s="36">
+      <c r="G16" s="57">
         <v>0.54876999999999998</v>
       </c>
-      <c r="G16" s="37">
+      <c r="H16" s="58">
         <v>5.262E-2</v>
       </c>
-      <c r="H16" s="28">
+      <c r="I16" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="53"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="15">
+    <row r="17" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="59">
         <v>1.64</v>
       </c>
-      <c r="E17" s="19">
+      <c r="F17" s="60">
         <v>0.22800000000000001</v>
       </c>
-      <c r="F17" s="20">
+      <c r="G17" s="61">
         <v>0.53088999999999997</v>
       </c>
-      <c r="G17" s="21">
+      <c r="H17" s="62">
         <v>4.1200000000000001E-2</v>
       </c>
-      <c r="H17" s="28">
+      <c r="I17" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="53"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="32" t="s">
+    <row r="18" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="34">
         <v>0.49299999999999999</v>
       </c>
-      <c r="E18" s="13">
+      <c r="F18" s="35">
         <v>5.5E-2</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G18" s="36">
         <v>0.68200000000000005</v>
       </c>
-      <c r="G18" s="17">
+      <c r="H18" s="37">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H18" s="28">
+      <c r="I18" s="5">
         <v>5</v>
       </c>
     </row>

</xml_diff>